<commit_message>
added image analysis to munging
</commit_message>
<xml_diff>
--- a/Project Documentation/Munging.xlsx
+++ b/Project Documentation/Munging.xlsx
@@ -5,16 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaryAlice\Documents\MDSI\STDS\Assignments\3MDL\AT2 - working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Assignment-2\Project Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{099E4476-C6BC-4B80-BB7C-3541436C17E9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55865B71-924A-4B75-8CE1-5F1FA3FAB07C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20406" windowHeight="4896" xr2:uid="{34F8C705-FA9D-4C44-818E-5C4837578CEA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="4890" activeTab="1" xr2:uid="{34F8C705-FA9D-4C44-818E-5C4837578CEA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tourism Data Analysis" sheetId="1" r:id="rId1"/>
+    <sheet name="Image Analysis" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Image Analysis'!$D$4:$G$59</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="69">
   <si>
     <t>Year</t>
   </si>
@@ -82,13 +87,163 @@
   </si>
   <si>
     <t>aggreagate(Bus + Emp)</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>picture_url</t>
+  </si>
+  <si>
+    <t>https://a0.muscache.com/im/pictures/778d441e-2c94-431a-8307-b32eaec69930.jpg</t>
+  </si>
+  <si>
+    <t>https://a0.muscache.com/im/pictures/3e9e50cf-2949-4a9e-9782-fecf327ea75a.jpg</t>
+  </si>
+  <si>
+    <t>https://a0.muscache.com/im/pictures/5946cfbc-af5a-492d-9aaa-a9db2fe35edc.jpg</t>
+  </si>
+  <si>
+    <t>https://a0.muscache.com/im/pictures/a3202371-a3b7-43b1-8cdc-404413db1d84.jpg</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>Park</t>
+  </si>
+  <si>
+    <t>Office Building</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>High Rise</t>
+  </si>
+  <si>
+    <t>Town</t>
+  </si>
+  <si>
+    <t>Urban</t>
+  </si>
+  <si>
+    <t>Downtown</t>
+  </si>
+  <si>
+    <t>Apartment Building</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Convention Center</t>
+  </si>
+  <si>
+    <t>Canal</t>
+  </si>
+  <si>
+    <t>Outdoors</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Waterfront</t>
+  </si>
+  <si>
+    <t>Harbor</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>Marina</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>Pool</t>
+  </si>
+  <si>
+    <t>Resort</t>
+  </si>
+  <si>
+    <t>Swimming Pool</t>
+  </si>
+  <si>
+    <t>Bedroom</t>
+  </si>
+  <si>
+    <t>Indoors</t>
+  </si>
+  <si>
+    <t>Interior Design</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Corridor</t>
+  </si>
+  <si>
+    <t>Furniture</t>
+  </si>
+  <si>
+    <t>Wall</t>
+  </si>
+  <si>
+    <t>Apartment</t>
+  </si>
+  <si>
+    <t>Dining Room</t>
+  </si>
+  <si>
+    <t>Kitchen</t>
+  </si>
+  <si>
+    <t>Dining Table</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>confidencelevel</t>
+  </si>
+  <si>
+    <t>FROM THIS</t>
+  </si>
+  <si>
+    <t>TO THIS</t>
+  </si>
+  <si>
+    <t>Count of context</t>
+  </si>
+  <si>
+    <t>has_building</t>
+  </si>
+  <si>
+    <t>has_high_rise</t>
+  </si>
+  <si>
+    <t>has_housing</t>
+  </si>
+  <si>
+    <t>has_city</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +279,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -151,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -167,6 +330,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,22 +648,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE4B9C12-9F46-4021-B611-4837593D3CBE}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="H21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.83984375" customWidth="1"/>
-    <col min="4" max="5" width="10.5234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="8.15625" customWidth="1"/>
-    <col min="10" max="10" width="11.3125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="19.05078125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -506,7 +671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,7 +715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2007</v>
       </c>
@@ -588,7 +753,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2007</v>
       </c>
@@ -626,7 +791,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2007</v>
       </c>
@@ -646,7 +811,7 @@
         <v>46532</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2007</v>
       </c>
@@ -666,7 +831,7 @@
         <v>54700</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2007</v>
       </c>
@@ -686,7 +851,7 @@
         <v>69037</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2007</v>
       </c>
@@ -706,7 +871,7 @@
         <v>64217</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2008</v>
       </c>
@@ -726,7 +891,7 @@
         <v>62751</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2008</v>
       </c>
@@ -746,7 +911,7 @@
         <v>63462</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2008</v>
       </c>
@@ -766,7 +931,7 @@
         <v>54700</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2008</v>
       </c>
@@ -786,7 +951,7 @@
         <v>69037</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2008</v>
       </c>
@@ -806,7 +971,7 @@
         <v>64217</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2008</v>
       </c>
@@ -826,7 +991,7 @@
         <v>62751</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -836,4 +1001,1107 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CBFCB1-6EC5-4844-8744-D358E18FC3D4}">
+  <dimension ref="A1:M59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="8" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>13467416</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>13467416</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>13467416</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>15882089</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>15882089</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>15882089</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>16197117</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>16197117</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>0.505</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>16197117</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>22298997</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>22298997</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>22298997</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>13467416</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>15882089</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>16197117</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11">
+        <v>0.505</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>22298997</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>16197117</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13">
+        <v>0.505</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>22298997</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>13467416</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>15882089</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>13467416</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>15882089</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18">
+        <v>0.51</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>13467416</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>15882089</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>13467416</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>15882089</v>
+      </c>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>13467416</v>
+      </c>
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>15882089</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>16197117</v>
+      </c>
+      <c r="E25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>22298997</v>
+      </c>
+      <c r="E26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>13467416</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>15882089</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28">
+        <v>0.52</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>16197117</v>
+      </c>
+      <c r="E29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>22298997</v>
+      </c>
+      <c r="E30" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>16197117</v>
+      </c>
+      <c r="E31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>22298997</v>
+      </c>
+      <c r="E32" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>13467416</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>15882089</v>
+      </c>
+      <c r="E34" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>16197117</v>
+      </c>
+      <c r="E35" t="s">
+        <v>51</v>
+      </c>
+      <c r="F35">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>22298997</v>
+      </c>
+      <c r="E36" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>13467416</v>
+      </c>
+      <c r="E37" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>15882089</v>
+      </c>
+      <c r="E38" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>13467416</v>
+      </c>
+      <c r="E39" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>15882089</v>
+      </c>
+      <c r="E40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>16197117</v>
+      </c>
+      <c r="E41" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>15882089</v>
+      </c>
+      <c r="E42" t="s">
+        <v>37</v>
+      </c>
+      <c r="F42">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>16197117</v>
+      </c>
+      <c r="E43" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>22298997</v>
+      </c>
+      <c r="E44" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>22298997</v>
+      </c>
+      <c r="E45" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>15882089</v>
+      </c>
+      <c r="E46" t="s">
+        <v>41</v>
+      </c>
+      <c r="F46">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>15882089</v>
+      </c>
+      <c r="E47" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>22298997</v>
+      </c>
+      <c r="E48" t="s">
+        <v>57</v>
+      </c>
+      <c r="F48">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>15882089</v>
+      </c>
+      <c r="E49" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>15882089</v>
+      </c>
+      <c r="E50" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>13467416</v>
+      </c>
+      <c r="E51" t="s">
+        <v>27</v>
+      </c>
+      <c r="F51">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>15882089</v>
+      </c>
+      <c r="E52" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>15882089</v>
+      </c>
+      <c r="E53" t="s">
+        <v>42</v>
+      </c>
+      <c r="F53">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>15882089</v>
+      </c>
+      <c r="E54" t="s">
+        <v>46</v>
+      </c>
+      <c r="F54">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>15882089</v>
+      </c>
+      <c r="E55" t="s">
+        <v>47</v>
+      </c>
+      <c r="F55">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>22298997</v>
+      </c>
+      <c r="E56" t="s">
+        <v>59</v>
+      </c>
+      <c r="F56">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>16197117</v>
+      </c>
+      <c r="E57" t="s">
+        <v>54</v>
+      </c>
+      <c r="F57">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>15882089</v>
+      </c>
+      <c r="E58" t="s">
+        <v>39</v>
+      </c>
+      <c r="F58">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>15882089</v>
+      </c>
+      <c r="E59" t="s">
+        <v>40</v>
+      </c>
+      <c r="F59">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="D4:G59" xr:uid="{53B83622-FC6E-473D-961D-DB2169FC7E0A}">
+    <sortState ref="D5:G59">
+      <sortCondition descending="1" ref="G4:G59"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5832A33-4FA8-476B-A3E6-EBB33F2FA9EA}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>13467416</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>15882089</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>0.96199999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>16197117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>0.505</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>22298997</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>0.79800000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>13467416</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>15882089</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>0.96199999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>16197117</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <v>0.505</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>22298997</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>0.79800000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>16197117</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10">
+        <v>0.505</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>22298997</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11">
+        <v>0.79800000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>13467416</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12">
+        <v>0.54700000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>15882089</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <v>0.51100000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13467416</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>